<commit_message>
Fix: removed extra text from dashboard
</commit_message>
<xml_diff>
--- a/Student_Performance_Dashboard.xlsx
+++ b/Student_Performance_Dashboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc11d47c0e4faea7/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarwa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF2EA2A2-B684-4799-8281-984438E6DC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEE4FE4-6068-447D-8BCD-9D55E7E6C0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{060C1504-875B-4DC9-903A-EE4B2C38CF48}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="21600" windowHeight="11100" activeTab="2" xr2:uid="{060C1504-875B-4DC9-903A-EE4B2C38CF48}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw_Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <definedName name="Slicer_Dept">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
       <x14:pivotCaches>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="81">
   <si>
     <t>ID</t>
   </si>
@@ -298,9 +297,6 @@
   </si>
   <si>
     <t>Grade</t>
-  </si>
-  <si>
-    <t>ss</t>
   </si>
 </sst>
 </file>
@@ -3951,8 +3947,8 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>182879</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="9" name="Dept 1">
@@ -3975,7 +3971,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -6059,7 +6055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B4B236-7C32-4025-875A-666C61C03341}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
@@ -7196,23 +7192,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC938389-CFD3-4890-82A6-D447DB6C6606}">
-  <dimension ref="N42"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="42" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N42" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <extLst>

</xml_diff>